<commit_message>
Joined Create & Index Views
</commit_message>
<xml_diff>
--- a/GuestBook/myLogger.xlsx
+++ b/GuestBook/myLogger.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>DateTime</t>
   </si>
@@ -428,6 +428,108 @@
   </si>
   <si>
     <t>Пользователь User 1 написал сообщение юзер 2 сообщение 1</t>
+  </si>
+  <si>
+    <t>2024-07-16 20:38:36</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 не удалось отправить сообщение</t>
+  </si>
+  <si>
+    <t>2024-07-16 20:38:45</t>
+  </si>
+  <si>
+    <t>2024-07-16 20:38:47</t>
+  </si>
+  <si>
+    <t>2024-07-16 20:38:55</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 вошёл в систему (log in)</t>
+  </si>
+  <si>
+    <t>2024-07-16 20:38:56</t>
+  </si>
+  <si>
+    <t>2024-07-16 20:39:03</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 2: фкфукефкефке</t>
+  </si>
+  <si>
+    <t>2024-07-17 22:59:12</t>
+  </si>
+  <si>
+    <t>2024-07-17 22:59:14</t>
+  </si>
+  <si>
+    <t>2024-07-17 22:59:20</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1: 12312313</t>
+  </si>
+  <si>
+    <t>2024-07-17 22:59:44</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:02:22</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:33:52</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:34:03</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:34:31</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:36:14</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:36:29</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:55:16</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:55:24</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1:123123</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:56:54</t>
+  </si>
+  <si>
+    <t>2024-07-17 23:57:08</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1: 22222</t>
+  </si>
+  <si>
+    <t>2024-07-18 00:07:01</t>
+  </si>
+  <si>
+    <t>2024-07-18 00:13:24</t>
+  </si>
+  <si>
+    <t>2024-07-18 00:19:58</t>
+  </si>
+  <si>
+    <t>2024-07-18 00:20:13</t>
+  </si>
+  <si>
+    <t>2024-07-18 00:20:20</t>
+  </si>
+  <si>
+    <t>2024-07-18 00:20:22</t>
+  </si>
+  <si>
+    <t>2024-07-18 00:20:33</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 2: 2312323231</t>
   </si>
 </sst>
 </file>
@@ -777,7 +879,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B393"/>
+  <dimension ref="A1:B420"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -3932,6 +4034,222 @@
         <v>135</v>
       </c>
     </row>
+    <row r="394">
+      <c r="A394" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B394" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B395" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B396" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B397" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B398" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B399" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B400" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B401" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B402" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B403" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B404" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B405" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B406" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B407" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B408" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B409" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B410" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B411" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B412" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B413" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B414" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B415" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B416" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B417" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B418" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B419" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B420" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Corrected the functionality of the application
</commit_message>
<xml_diff>
--- a/GuestBook/myLogger.xlsx
+++ b/GuestBook/myLogger.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="264">
   <si>
     <t>DateTime</t>
   </si>
@@ -530,6 +530,288 @@
   </si>
   <si>
     <t>Пользователь User 2 написал сообщение 2: 2312323231</t>
+  </si>
+  <si>
+    <t>2024-07-18 10:43:22</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 2; 33333</t>
+  </si>
+  <si>
+    <t>2024-07-18 10:43:41</t>
+  </si>
+  <si>
+    <t>2024-07-18 10:47:13</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 2: 33333</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:09:37</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 2:23231</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:09:49</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:10:00</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 вышел из системы (logout)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:10:27</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:14:23</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:15:25</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:17:03</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:22:54</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:24:11</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:24:45</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:25:33</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:25:36</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:26:06</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:26:16</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:26:28</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1:7777777</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:26:56</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:27:11</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:28:19</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:28:32</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:28:39</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:28:58</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1: вапвапвап</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:34:52</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:35:00</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:35:07</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:35:33</t>
+  </si>
+  <si>
+    <t>Пользователь User 15 успешно прошёл регистрацию)</t>
+  </si>
+  <si>
+    <t>Пользователь User 15 вошёл в систему (cookie value)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:35:50</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 15: ррркнуг</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:36:19</t>
+  </si>
+  <si>
+    <t>Пользователь User 15 вышел из системы (logout)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:39:04</t>
+  </si>
+  <si>
+    <t>Пользователь User 16 успешно прошёл регистрацию)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:39:16</t>
+  </si>
+  <si>
+    <t>Пользователь User 16 вошёл в систему (cookie value)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:39:27</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 16: вапвпвпа</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:39:41</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:39:46</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 16: кенкен</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:39:58</t>
+  </si>
+  <si>
+    <t>Пользователь User 16 вышел из системы (logout)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:07</t>
+  </si>
+  <si>
+    <t>Пользователь User 16 вошёл в систему (log in)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:10</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:14</t>
+  </si>
+  <si>
+    <t>Пользователь User 16 написал сообщение 16 кенкен</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:25</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:31</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:37</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:43</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1 кеуке</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:49</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:40:58</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:41:12</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:42:18</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:42:26</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:42:31</t>
+  </si>
+  <si>
+    <t>Пользователь User 2 написал сообщение 2 кн</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:42:44</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:42:55</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:43:01</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:43:07</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1 вапро</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:43:22</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:43:27</t>
+  </si>
+  <si>
+    <t>Пользователь User 1 написал сообщение 1 ыкне</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:43:33</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:43:45</t>
+  </si>
+  <si>
+    <t>Пользователь User 17 успешно прошёл регистрацию)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:44:01</t>
+  </si>
+  <si>
+    <t>Пользователь User 17 вошёл в систему (cookie value)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:44:50</t>
+  </si>
+  <si>
+    <t>Пользователь User 17 вышел из системы (logout)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:45:18</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:45:29</t>
+  </si>
+  <si>
+    <t>Пользователь User 18 успешно прошёл регистрацию)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:45:41</t>
+  </si>
+  <si>
+    <t>Пользователь User 18 вошёл в систему (log in)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:45:45</t>
+  </si>
+  <si>
+    <t>Пользователь User 18 вошёл в систему (cookie value)</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:45:53</t>
+  </si>
+  <si>
+    <t>Пользователь User 18 написал сообщение 18: врповпрвпр</t>
+  </si>
+  <si>
+    <t>2024-07-18 11:46:38</t>
+  </si>
+  <si>
+    <t>Пользователь User 18 вышел из системы (logout)</t>
   </si>
 </sst>
 </file>
@@ -879,7 +1161,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B420"/>
+  <dimension ref="A1:B486"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -4250,6 +4532,534 @@
         <v>169</v>
       </c>
     </row>
+    <row r="421">
+      <c r="A421" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B421" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B422" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B423" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B424" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B425" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B426" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B427" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B428" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B429" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B430" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B431" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B432" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B433" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B434" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B435" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B436" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B437" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B438" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B439" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B440" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B441" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B442" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B443" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B444" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B445" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B446" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B447" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B448" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B449" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B450" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B451" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B452" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B453" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B454" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B455" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B456" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B457" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B458" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B459" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B460" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B461" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B462" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B463" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B464" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="B465" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B466" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B467" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B468" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B469" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B470" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B471" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B472" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="B473" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B475" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="B476" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B477" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B478" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B481" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B482" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B483" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B484" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B485" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B486" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>